<commit_message>
All changes through Sep092024
</commit_message>
<xml_diff>
--- a/DataLoads/Output/DatabaseDownloadTransactionsTmp.xlsx
+++ b/DataLoads/Output/DatabaseDownloadTransactionsTmp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,16 +508,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-07-30</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RECURRING PAYMENT AUTHORIZED ON 07/29 DNH*GODADDY#321752 480-5058855 AZ S304211626202408 CARD 4162</t>
+          <t>OnePlus Realty G SIGONFILE 083024 5CCJP2 Midway Inn LLC</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-204.42</v>
+        <v>16702.38</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -536,17 +536,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>Midway</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -556,12 +556,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>Internet</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
@@ -573,16 +573,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-07-30</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Instant Pmt from ONEPLUS REALTY GROUP LLC on 07/30 Ref#20240730021000021P1BRJPC00520076928</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PF28CZK TRULO MONTHLY PM FEE MIDWAY INN</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>17028.44</v>
+        <v>-1500</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -601,19 +601,19 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>W9-TRULO</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>Midway</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>W9-ONEPLUS</t>
-        </is>
-      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>Initial</t>
@@ -621,12 +621,12 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
@@ -638,16 +638,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-07-23</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CHECK # 1011</t>
+          <t>Instant Pmt from ONEPLUS REALTY GROUP LLC on 08/30 Ref#20240830021000021P1BRJPC03760121683</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-800</v>
+        <v>920</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -661,37 +661,37 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>B01-SecurityDeposit</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Security-Refund</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>Midway</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>ChristinaFain</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
@@ -703,16 +703,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-07-22</t>
+          <t>2024-08-13</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>WF Bus Credit AUTO PAY 240721 90469914333885 GUPTA,NEERAJ</t>
+          <t>RECURRING PAYMENT AUTHORIZED ON 08/12 Spectrum 855-707-7328 MO S464225547250464 CARD 4162</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>-136.07</v>
+        <v>-83.29000000000001</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Exp-Repair</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>Autopay</t>
+          <t>Internet</t>
         </is>
       </c>
     </row>
@@ -768,16 +768,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-07-22</t>
+          <t>2024-08-14</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Instant Pmt from ONEPLUS REALTY GROUP LLC on 07/21 Ref#20240721021000021P1BRJPC00510064841</t>
+          <t>Instant Pmt from ONEPLUS REALTY GROUP LLC on 08/14 Ref#20240814021000021P1BRJPC00500037215</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>800</v>
+        <v>250</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -833,16 +833,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>2024-08-06</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>RECURRING PAYMENT AUTHORIZED ON 07/14 DNH*GODADDY#318938 480-5058855 AZ S584196656484877 CARD 4162</t>
+          <t>BUSINESS TO BUSINESS ACH Lument7313 ACH 490011466</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-22.17</v>
+        <v>-9368.889999999999</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -886,28 +886,28 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Internet</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-07-15</t>
+          <t>2024-09-06</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RECURRING PAYMENT AUTHORIZED ON 07/12 Spectrum 855-707-7328 MO S584194554099969 CARD 4162</t>
+          <t>BILL PAY Eddy Account 9189321 ON-LINE xxxx xxxxxxxxxx xroup ON 09-06</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-77.28</v>
+        <v>-1894.9</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -926,7 +926,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -946,12 +946,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>EddyEstatesLLC</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>Internet</t>
+          <t>1905Morning</t>
         </is>
       </c>
     </row>
@@ -963,16 +963,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-07-11</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BUSINESS TO BUSINESS ACH CITY OFARLINGTON UTILITYIVR 240710 5743289 MIDWAY INN *LLC</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VK6BX TRULO MONTHLY PM FEE MIDWAY INN</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-956.2</v>
+        <v>-1500</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -991,12 +991,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1011,33 +1011,33 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>CityServices</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>108Meadow</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-07-08</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>BUSINESS TO BUSINESS ACH Lument7313 ACH 490011466</t>
+          <t>SERVICEMAC PMT MTGE PAYMT 090124 5114002632 PARUL GUPTA</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-9212.299999999999</v>
+        <v>-748.9299999999999</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>108Meadow</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1088,21 +1088,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-07-08</t>
+          <t>2024-08-27</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PURCHASE AUTHORIZED ON 07/06 Mobimatter Abu Dhabi ARE S464188635540782 CARD 4162</t>
+          <t>BILL PAY Eddy Account 9189321 ON-LINE xxxx xxxxxxxxxx xroup ON 08-27</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-11.63</v>
+        <v>-947</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Exp-Travel</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1131,43 +1131,43 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>VivekPersonal</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>EddyEstatesLLC</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>1905Morning</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-26</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ5FSZ3 TRULO MONTHLY PM FEE MIDWAY INN</t>
+          <t>ONLINE TRANSFER FROM GUPTA P REF #IB0PC4CFZC PLATINUM SAVINGS EDDY ESTATES LLC MORTGAGE PAYMENT</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>-1500</v>
+        <v>947</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1186,17 +1186,17 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1206,12 +1206,12 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>EddyEstatesLLC</t>
         </is>
       </c>
     </row>
@@ -1288,12 +1288,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VCNRL 108MV TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PF25M6M 108MV TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1348,21 +1348,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>108Meadow</t>
+          <t>116Meadow</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SERVICEMAC PMT MTGE PAYMT 070124 5114002632 PARUL GUPTA</t>
+          <t>NEWREZ-SHELLPOIN ACH PMT 240831 0683624456 GUPTA PARUL</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>-748.9299999999999</v>
+        <v>-456.02</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>108Meadow</t>
+          <t>116Meadow</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1418,12 +1418,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ58NCB 108MV TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VCNRL 108MV TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1548,12 +1548,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2V3PQ8 116MV TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PDZVTSM 116MV TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1613,16 +1613,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 071024 4TRBL2 Meadow View Homes LLC</t>
+          <t>RECURRING TRANSFER TO MEADOW VIEW HOMES LLC REF #OP0P5LXJ2X BUSINESS MARKET RATE SAVINGS 116 MV CHK TO SAV</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1600</v>
+        <v>-150</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1636,24 +1636,24 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>A01-Income</t>
+          <t>F01-BankTransfer</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Transfer</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
+          <t>GeneralVendor</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
           <t>116Meadow</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>W9-ONEPLUS</t>
-        </is>
-      </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>Initial</t>
@@ -1661,12 +1661,12 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>Checking</t>
         </is>
       </c>
     </row>
@@ -1678,16 +1678,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-07-09</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO MEADOW VIEW HOMES LLC REF #OP0NSR3SBH BUSINESS MARKET RATE SAVINGS 116 MV CHK TO SAV</t>
+          <t>OnePlus Realty G SIGONFILE 080924 WY88N2 Meadow View Homes LLC</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>-150</v>
+        <v>1900</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1701,22 +1701,22 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>F01-BankTransfer</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Transfer</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>116Meadow</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>116Meadow</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1726,33 +1726,33 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>Checking</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>116Meadow</t>
+          <t>2208Chase</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NEWREZ-SHELLPOIN ACH PMT 240630 0683624456 GUPTA PARUL</t>
+          <t>INTEREST PAYMENT</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>-456.02</v>
+        <v>0.01</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1771,17 +1771,17 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Rev-Interest</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>2208Chase</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>116Meadow</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1791,12 +1791,12 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>BankInterest</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
     </row>
@@ -1808,12 +1808,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ6F5RZ 116MV TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2V3PQ8 116MV TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1868,21 +1868,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2208Chase</t>
+          <t>1342Newton</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>INTEREST PAYMENT</t>
+          <t>NEWREZ-SHELLPOIN ACH PMT 240831 0683856942 GUPTA PARUL</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.01</v>
+        <v>-563.38</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1901,17 +1901,17 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Rev-Interest</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2208Chase</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>1342Newton</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1921,12 +1921,12 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>BankInterest</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
@@ -2003,12 +2003,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VKXGK NEWTON TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PF223XX NEWTON TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2063,21 +2063,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1342Newton</t>
+          <t>1316Rosemon</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 073124 RZKLM2 Pagoda Homes (Newton)</t>
+          <t>PENNYMAC CASH Sep 24 8028350915-0057 1316 Rosemon</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1748.17</v>
+        <v>-963.16</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -2096,17 +2096,17 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>1342Newton</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>1316Rosemon</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2116,12 +2116,12 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
@@ -2133,16 +2133,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 071024 5TRBL2 Pagoda Homes (Newton)</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VKXGK NEWTON TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>1995</v>
+        <v>-75</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -2161,19 +2161,19 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
+          <t>W9-TRULO</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
           <t>1342Newton</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>W9-ONEPLUS</t>
-        </is>
-      </c>
       <c r="K27" t="inlineStr">
         <is>
           <t>Initial</t>
@@ -2181,33 +2181,33 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1342Newton</t>
+          <t>1316Rosemon</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>NEWREZ-SHELLPOIN ACH PMT 240630 0683856942 GUPTA PARUL</t>
+          <t>OnePlus Realty G SIGONFILE 080924 YY88N2 Pagoda Homes LLC (Rose</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>-563.38</v>
+        <v>1883.52</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -2226,17 +2226,17 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>1316Rosemon</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1342Newton</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2246,12 +2246,12 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
@@ -2263,16 +2263,16 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-08-02</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>PENNYMAC CASH Aug 24 8028350915-0056 1316 Rosemon</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PDZ4CND ROSEMON TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>-963.16</v>
+        <v>-150</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -2291,12 +2291,12 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2311,12 +2311,12 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
@@ -2328,16 +2328,16 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-08-21</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TXGGY ROSEMON TO TRULO PROPERTY MANAGEMENT</t>
+          <t>FOREMOST EPM PYMT 240820 3810091873545 VIVEK JADHAV</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>-150</v>
+        <v>-395</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -2356,12 +2356,12 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Exp-Insurance</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2376,12 +2376,12 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>Insurance</t>
         </is>
       </c>
     </row>
@@ -2393,16 +2393,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
+          <t>2024-08-02</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>FOREMOST EPM PYMT 240726 3810091873545 VIVEK JADHAV</t>
+          <t>PENNYMAC CASH Aug 24 8028350915-0056 1316 Rosemon</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>-414</v>
+        <v>-963.16</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Exp-Insurance</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2446,28 +2446,28 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>Insurance</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1316Rosemon</t>
+          <t>104Meadow</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 071024 7TRBL2 Pagoda Homes LLC (Rose</t>
+          <t>PENNYMAC CASH Sep 24 8028352704-0057 104 Meadow</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3729</v>
+        <v>-730.2</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2486,17 +2486,17 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>1316Rosemon</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>104Meadow</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2506,12 +2506,12 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
@@ -2523,16 +2523,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-07-02</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PENNYMAC CASH Jul 24 8028350915-0055 1316 Rosemon</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TXGGY ROSEMON TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>-963.16</v>
+        <v>-150</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -2551,12 +2551,12 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2571,33 +2571,33 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1316Rosemon</t>
+          <t>104Meadow</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ54Y3C ROSEMON TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PDZPCHZ 104MV TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>-150</v>
+        <v>-75</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>1316Rosemon</t>
+          <t>104Meadow</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2648,21 +2648,21 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>104Meadow</t>
+          <t>Midway</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-08-02</t>
+          <t>2024-09-06</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PENNYMAC CASH Aug 24 8028352704-0056 104 Meadow</t>
+          <t>BUSINESS TO BUSINESS ACH Lument7313 ACH 490011466</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>-730.2</v>
+        <v>-9368.889999999999</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>104Meadow</t>
+          <t>Midway</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2718,16 +2718,16 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 071024 3TRBL2 Meadow View Homes LLC</t>
+          <t>OnePlus Realty G SIGONFILE 080924 VY88N2 Meadow View Homes LLC</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1300</v>
+        <v>1950</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -2778,21 +2778,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>104Meadow</t>
+          <t>116MeadowSavings</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-07-02</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PENNYMAC CASH Jul 24 8028352704-0055 104 Meadow</t>
+          <t>INTEREST PAYMENT</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>-730.2</v>
+        <v>0.02</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2811,17 +2811,17 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Rev-Interest</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>116MeadowSavings</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>104Meadow</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -2831,33 +2831,33 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>BankInterest</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>104Meadow</t>
+          <t>711Parks</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-09-06</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ55Y6Q 104MV TO TRULO PROPERTY MANAGEMENT</t>
+          <t>OnePlus Realty G SIGONFILE 090624 S8NWP2 Pagoda Homes LLC (711</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>-75</v>
+        <v>998.5700000000001</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2876,17 +2876,17 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>711Parks</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>104Meadow</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -2896,12 +2896,12 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
@@ -2913,16 +2913,16 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>INTEREST PAYMENT</t>
+          <t>RECURRING TRANSFER FROM MEADOW VIEW HOMES LLC REF #OP0P5LXJ2X BUSINESS CHECKING 116 MV CHK TO SAV</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.03</v>
+        <v>150</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2936,12 +2936,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>A01-Income</t>
+          <t>F01-BankTransfer</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Rev-Interest</t>
+          <t>Transfer</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>BankInterest</t>
+          <t>Savings</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -2973,21 +2973,21 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>116MeadowSavings</t>
+          <t>711Parks</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-07-09</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER FROM MEADOW VIEW HOMES LLC REF #OP0NSR3SBH BUSINESS CHECKING 116 MV CHK TO SAV</t>
+          <t>SERVICEMAC PMT MTGE PAYMT 090124 5114002634 PARUL GUPTA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>150</v>
+        <v>-733.95</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -3001,22 +3001,22 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>F01-BankTransfer</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Transfer</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>116MeadowSavings</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>711Parks</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3026,12 +3026,12 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Savings</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
@@ -3108,12 +3108,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TT3W6 PARKS TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PF2B27T PARKS TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -3168,21 +3168,21 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>711Parks</t>
+          <t>108Pagoda</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SERVICEMAC PMT MTGE PAYMT 070124 5114002634 PARUL GUPTA</t>
+          <t>FREEDOM MTG PYMTS 090224 0129201927 NEERAJ GUPTA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>-733.95</v>
+        <v>-726.97</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -3211,7 +3211,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>711Parks</t>
+          <t>108Pagoda</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3238,12 +3238,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ5P3GX PARKS TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TT3W6 PARKS TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -3368,12 +3368,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VHFSF TRULO PROPERTY MANAGEMENT MONTHLY FEE</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PDYWQYM TRULO PROPERTY MANAGEMENT MONTHLY FEE</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -3433,16 +3433,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 071024 6TRBL2 Pagoda Homes LLC (108</t>
+          <t>OnePlus Realty G SIGONFILE 080924 XY88N2 Pagoda Homes LLC (108</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>1925</v>
+        <v>2025</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -3493,21 +3493,21 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>108Pagoda</t>
+          <t>2417Garden</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>FREEDOM MTG PYMTS 070124 0129201927 NEERAJ GUPTA</t>
+          <t>JPMORGAN CHASE CHASE ACH 090124 4027425045 MEADOW VIEW HOMES LLC</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>-726.97</v>
+        <v>-947.72</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -3536,7 +3536,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>108Pagoda</t>
+          <t>2417Garden</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -3563,12 +3563,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ59FR9 TRULO PROPERTY MANAGEMENT MONTHLY FEE</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VHFSF TRULO PROPERTY MANAGEMENT MONTHLY FEE</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -3628,16 +3628,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>JPMORGAN CHASE CHASE ACH 080124 4027425045 MEADOW VIEW HOMES LLC</t>
+          <t>INTEREST PAYMENT</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>-947.72</v>
+        <v>0.1</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -3656,17 +3656,17 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Rev-Interest</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>2417Garden</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>2417Garden</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -3676,12 +3676,12 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>BankInterest</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
     </row>
@@ -3693,16 +3693,16 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>INTEREST PAYMENT</t>
+          <t>JPMORGAN CHASE CHASE ACH 080124 4027425045 MEADOW VIEW HOMES LLC</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.08</v>
+        <v>-947.72</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -3721,19 +3721,19 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Rev-Interest</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
+          <t>GeneralVendor</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
           <t>2417Garden</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>GeneralCustomer</t>
-        </is>
-      </c>
       <c r="K51" t="inlineStr">
         <is>
           <t>Initial</t>
@@ -3741,12 +3741,12 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>BankInterest</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M51" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
@@ -3758,16 +3758,16 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 071024 1TRBL2 Meadow View Homes LLC</t>
+          <t>OnePlus Realty G SIGONFILE 080924 TY88N2 Meadow View Homes LLC</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>2700</v>
+        <v>2950</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -3818,21 +3818,21 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2417Garden</t>
+          <t>PagodaSecurity</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>JPMORGAN CHASE CHASE ACH 070124 4027425045 MEADOW VIEW HOMES LLC</t>
+          <t>INTEREST PAYMENT</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>-947.72</v>
+        <v>0.24</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -3851,17 +3851,17 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Rev-Interest</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>PagodaSecurity</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>2417Garden</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -3871,33 +3871,33 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>BankInterest</t>
         </is>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>PagodaSecurity</t>
+          <t>Partnership</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-09-05</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>INTEREST PAYMENT</t>
+          <t>ONLINE TRANSFER TO MEADOW VIEW HOMES LLC REF #IB0PGKBTSH BUSINESS CHECKING EDDY ESTATES JUL AUG MORTGAGE</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0.24</v>
+        <v>-1894.9</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -3916,17 +3916,17 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Rev-Interest</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>PagodaSecurity</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>Partnership</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -3936,12 +3936,12 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>BankInterest</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>EddyEstatesLLC</t>
         </is>
       </c>
     </row>
@@ -3953,7 +3953,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-30</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3962,7 +3962,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>158.77</v>
+        <v>121.69</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -4013,21 +4013,21 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>1117Brewer</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2024-07-12</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ZELLE TO PROPERTY MANAGEMENT TRULO ON 07/12 REF #RP0SF2YHM4 ATTORNEY FEE WIRE THRU CHASE FOR CHAKRI</t>
+          <t>SERVICEMAC PMT MTGE PAYMT 090124 5114002633 PARUL GUPTA</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>-450</v>
+        <v>-711.48</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -4041,27 +4041,27 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>C01-Capex</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Capex-Refi</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>1117Brewer</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>HardmoneyChakri</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -4071,7 +4071,7 @@
       </c>
       <c r="M56" t="inlineStr">
         <is>
-          <t>HardmoneyChakri</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
@@ -4083,16 +4083,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2024-07-12</t>
+          <t>2024-08-26</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>ONLINE TRANSFER TO GUPTA N REF #IB0NTSRLJC EVERYDAY CHECKING CHAKRI WIRE XFER FEE</t>
+          <t>ONLINE TRANSFER TO MEADOW VIEW HOMES LLC REF #IB0PC4CFZC BUSINESS CHECKING EDDY ESTATES LLC MORTGAGE PAYMENT</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>-40</v>
+        <v>-947</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -4106,12 +4106,12 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>C01-Capex</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Capex-Refi</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -4126,38 +4126,38 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>HardmoneyChakri</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M57" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>EddyEstatesLLC</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>1117Brewer</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2024-07-12</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>ONLINE TRANSFER FROM GUPTA N REF #IB0NTSQSGR EVERYDAY CHECKING CHAKRI PAID ATTORNEY FEE</t>
+          <t>SERVICEMAC PMT MTGE PAYMT 080124 5114002633 PARUL GUPTA</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>450</v>
+        <v>-711.48</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -4171,58 +4171,58 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>C01-Capex</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Capex-Refi</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>1117Brewer</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>HardmoneyChakri</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>1117Brewer</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2024-07-12</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ONLINE TRANSFER FROM GUPTA N REF #IB0NTSQG3V EVERYDAY CHECKING CHAKRI INT JULY</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PF23MNH BREWER TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>1100</v>
+        <v>-75</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -4236,58 +4236,58 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>C01-Capex</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Capex-Refi</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>1117Brewer</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>HardmoneyChakri</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ONLINE TRANSFER TO GUPTA N REF #IB0NT79WFZ EVERYDAY CHECKING CHAKRI AND SRAVYA</t>
+          <t>PENNYMAC CASH Sep 24 8028351602-0056 vivek jadhav</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>-135000</v>
+        <v>-694.01</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -4301,12 +4301,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>C01-Capex</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Capex-Refi</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -4316,43 +4316,43 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>HardmoneyChakri</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>1117Brewer</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ONLINE TRANSFER TO GUPTA N REF #IB0NT74JWP EVERYDAY CHECKING CHAKRADER AND SRAVYA</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TWZK5 BREWER TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>-15000</v>
+        <v>-75</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -4366,58 +4366,58 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>C01-Capex</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Capex-Refi</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>1117Brewer</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>HardmoneyChakri</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M61" t="inlineStr">
         <is>
-          <t>Partnership</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-08-02</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SERVICEMAC PMT MTGE PAYMT 080124 5114002633 PARUL GUPTA</t>
+          <t>PENNYMAC CASH Aug 24 8028351602-0055 vivek jadhav</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>-711.48</v>
+        <v>-694.01</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -4468,17 +4468,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2TWZK5 BREWER TO TRULO PROPERTY MANAGEMENT</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0PDZTNSD WINTERGREEN TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -4511,7 +4511,7 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
@@ -4533,21 +4533,21 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 073124 PZKLM2 Neeraj Gupta (Brewer)</t>
+          <t>OnePlus Realty G SIGONFILE 080924 1Z88N2 Pagoda Homes (Wintergr</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>2295</v>
+        <v>1900</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -4571,7 +4571,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
@@ -4598,21 +4598,21 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-29</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 071024 0TRBL2 Neeraj Gupta (Brewer)</t>
+          <t>ORIG CO NAME:CHASE CREDIT CRD       ORIG ID:4760039224 DESC DATE:240828 CO ENTRY DESCR:AUTOPAYBUSSEC:PPD    TRACE#:021000025701084 EED:240829   IND ID:                             IND NAME:GUPTA NEERAJ TRN: 2425701084TC</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>1823.14</v>
+        <v>-40.35</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -4631,17 +4631,17 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-Repair</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>Common</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
@@ -4651,33 +4651,33 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>Autopay</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SERVICEMAC PMT MTGE PAYMT 070124 5114002633 PARUL GUPTA</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2V8M6F WINTERGREEN TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>-711.48</v>
+        <v>-75</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -4696,17 +4696,17 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>874Wintergreen</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -4716,33 +4716,33 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2024-08-02</t>
+          <t>2024-09-06</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>PENNYMAC CASH Aug 24 8028351602-0055 vivek jadhav</t>
+          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240905 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000017273186 EED:240906   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2507273186TC</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>-694.01</v>
+        <v>-45.66</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -4761,7 +4761,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -4786,28 +4786,28 @@
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>CityServices</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>104Meadow</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-08-02</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2V8M6F WINTERGREEN TO TRULO PROPERTY MANAGEMENT</t>
+          <t>PENNYMAC CASH Aug 24 8028352704-0056 104 Meadow</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>-75</v>
+        <v>-730.2</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -4826,17 +4826,17 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>104Meadow</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -4846,33 +4846,33 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>OnePlus Realty G SIGONFILE 071024 BTRBL2 Pagoda Homes (Wintergr</t>
+          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240902 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000014168270 EED:240903   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2474168270TC</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>1900</v>
+        <v>-85.56</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -4891,17 +4891,17 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -4911,33 +4911,33 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>Energy</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2024-07-02</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PENNYMAC CASH Jul 24 8028351602-0054 vivek jadhav</t>
+          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240902 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000014168302 EED:240903   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2474168302TC</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>-694.01</v>
+        <v>-125.78</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -4956,7 +4956,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -4966,7 +4966,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -4981,28 +4981,28 @@
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>Energy</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-13</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ68C2D WINTERGREEN TO TRULO PROPERTY MANAGEMENT</t>
+          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240812 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000012973937 EED:240813   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2262973937TC</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>-75</v>
+        <v>-178.76</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -5021,17 +5021,17 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>874Wintergreen</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5041,33 +5041,33 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>CityServices</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-29</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Online Transfer from CHK ...6571 transaction#: 21572783954</t>
+          <t>Online Payment 21567571562 To CHASE HOME MORTGAGE 08/29</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>248</v>
+        <v>-1118.25</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -5081,58 +5081,58 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>F01-BankTransfer</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Transfer</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Common-&gt;Canoga</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Zelle payment from TRULO PROPERTY MANAGEMENT LLC 21572866504</t>
+          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240808 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000012459473 EED:240809   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2222459473TC</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>250</v>
+        <v>-45.66</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -5151,17 +5151,17 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Exp-Repair</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5171,33 +5171,33 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>TRULORefund</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M73" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>CityServices</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:CHASE CREDIT CRD       ORIG ID:4760039224 DESC DATE:240728 CO ENTRY DESCR:AUTOPAYBUSSEC:PPD    TRACE#:021000024987396 EED:240729   IND ID:                             IND NAME:GUPTA NEERAJ TRN: 2114987396TC</t>
+          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240808 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000012459467 EED:240809   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2222459467TC</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>-358.39</v>
+        <v>-48.89</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -5216,7 +5216,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Exp-Repair</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -5226,7 +5226,7 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
@@ -5241,28 +5241,28 @@
       </c>
       <c r="M74" t="inlineStr">
         <is>
-          <t>Autopay</t>
+          <t>CityServices</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:CHASE CREDIT CRD       ORIG ID:4760039224 DESC DATE:240628 CO ENTRY DESCR:AUTOPAYBUSSEC:PPD    TRACE#:021000020238031 EED:240701   IND ID:                             IND NAME:GUPTA NEERAJ TRN: 1830238031TC</t>
+          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240808 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000012459469 EED:240809   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2222459469TC</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>-96.29000000000001</v>
+        <v>-65.56</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -5281,7 +5281,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Exp-Repair</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -5291,7 +5291,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Common</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -5306,28 +5306,28 @@
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>Autopay</t>
+          <t>CityServices</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7417Canoga</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-06</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Online Transfer to CHK ...5031 transaction#: 21572783954 07/31</t>
+          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240805 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000017379970 EED:240806   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2197379970TC</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>-248</v>
+        <v>-82.47</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -5341,12 +5341,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>F01-BankTransfer</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Transfer</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -5356,22 +5356,22 @@
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>7417Canoga</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Common-&gt;Canoga</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>7417Canoga</t>
+          <t>Energy</t>
         </is>
       </c>
     </row>
@@ -5383,16 +5383,16 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-06</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Online Payment 21229559529 To CHASE HOME MORTGAGE 07/31</t>
+          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240805 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000017363565 EED:240806   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2197363565TC</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>-1118.25</v>
+        <v>-119.6</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -5411,7 +5411,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -5436,7 +5436,7 @@
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>Energy</t>
         </is>
       </c>
     </row>
@@ -5448,16 +5448,16 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2024-07-29</t>
+          <t>2024-08-06</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t xml:space="preserve">CHECK 2032  </t>
+          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240805 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000017363592 EED:240806   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2197363592TC</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>-500</v>
+        <v>-188.8</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -5471,12 +5471,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>B01-SecurityDeposit</t>
+          <t>A01-Income</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Security-Refund</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -5491,17 +5491,17 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Adriana</t>
+          <t>Initial</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Initial</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>Energy</t>
         </is>
       </c>
     </row>
@@ -5513,16 +5513,16 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-05</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240709 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018411692 EED:240710   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1928411692TC</t>
+          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240802 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000016012185 EED:240805   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2186012185TC</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>-46.3</v>
+        <v>-169.1</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -5566,28 +5566,28 @@
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>CityServices</t>
+          <t>Energy</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>4920Brianhill</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240709 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018411685 EED:240710   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1928411685TC</t>
+          <t>ORIG CO NAME:JPMORGAN CHASE         ORIG ID:1000008113 DESC DATE:090124 CO ENTRY DESCR:CHASE ACH SEC:PPD    TRACE#:021000023949858 EED:240903   IND ID:                             IND NAME:MEADOW VIEW HOMES LLC TRN: 2473949858TC</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>-49.54</v>
+        <v>-1383.06</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -5606,7 +5606,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -5616,7 +5616,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>4920Brianhill</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -5631,28 +5631,28 @@
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>CityServices</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>4920Brianhill</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240709 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018411691 EED:240710   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1928411691TC</t>
+          <t>ORIG CO NAME:JPMORGAN CHASE         ORIG ID:1000008113 DESC DATE:080124 CO ENTRY DESCR:CHASE ACH SEC:PPD    TRACE#:021000029832472 EED:240801   IND ID:                             IND NAME:MEADOW VIEW HOMES LLC TRN: 2149832472TC</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>-70.08</v>
+        <v>-1383.06</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -5671,7 +5671,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>4920Brianhill</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -5696,28 +5696,28 @@
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>CityServices</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>4920Brianhill</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-15</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240709 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000018411687 EED:240710   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1928411687TC</t>
+          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:081524 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926085820470 EED:240815   IND ID:WCRRN2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 2285820470TC</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>-134.46</v>
+        <v>4400</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -5736,17 +5736,17 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>4920Brianhill</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -5756,33 +5756,33 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
         <is>
-          <t>CityServices</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>8604Wagon</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:071024 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088315743 EED:240710   IND ID:2TRBL2                       IND NAME:Pagoda Homes LLC (Jame                                                                                       469-867-9837 TRN: 1928315743TC</t>
+          <t>ORIG CO NAME:PENNYMAC               ORIG ID:1262049351 DESC DATE:Sep 24 CO ENTRY DESCR:CASH      SEC:WEB    TRACE#:021000024465512 EED:240903   IND ID:8028351082-0057              IND NAME:8604 Wagon TRN: 2474465512TC</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>1504.75</v>
+        <v>-843.79</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -5801,17 +5801,17 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>8604Wagon</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -5821,33 +5821,33 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>8604Wagon</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2024-07-03</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240702 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000010929691 EED:240703   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1850929691TC</t>
+          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:080924 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926082370598 EED:240809   IND ID:0Z88N2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 2222370598TC</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>-51.49</v>
+        <v>1814.38</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -5866,17 +5866,17 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>8604Wagon</t>
         </is>
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -5886,33 +5886,33 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>Energy</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>8604Wagon</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2024-07-03</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240702 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000010926310 EED:240703   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1850926310TC</t>
+          <t>ORIG CO NAME:PENNYMAC               ORIG ID:1262049351 DESC DATE:Aug 24 CO ENTRY DESCR:CASH      SEC:WEB    TRACE#:021000021437718 EED:240801   IND ID:8028351082-0056              IND NAME:8604 Wagon TRN: 2141437718TC</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>-95.72</v>
+        <v>-843.79</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -5931,7 +5931,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>8604Wagon</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -5956,28 +5956,28 @@
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>Energy</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>114Sidney</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2024-07-03</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240702 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000010926327 EED:240703   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1850926327TC</t>
+          <t>ORIG CO NAME:SERVICEMAC PMT         ORIG ID:4823070213 DESC DATE:090124 CO ENTRY DESCR:MTGE PAYMTSEC:PPD    TRACE#:091000013573470 EED:240903   IND ID:                             IND NAME:PARUL GUPTA TRN: 2473573470TC</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>-143.42</v>
+        <v>-675.63</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -5996,7 +5996,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Exp-Utilities</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -6006,7 +6006,7 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>114Sidney</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6021,7 +6021,7 @@
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>Energy</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
@@ -6033,16 +6033,16 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2024-07-03</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240702 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000010929696 EED:240703   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 1850929696TC</t>
+          <t>ORIG CO NAME:EXELON CORPORATI       ORIG ID:0000000160 DESC DATE:240902 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000014168561 EED:240903   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2474168561TC</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>-148.43</v>
+        <v>-82.27</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -6093,21 +6093,21 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>4920Brianhill</t>
+          <t>Midway</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-06</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:JPMORGAN CHASE         ORIG ID:1000008113 DESC DATE:080124 CO ENTRY DESCR:CHASE ACH SEC:PPD    TRACE#:021000029832472 EED:240801   IND ID:                             IND NAME:MEADOW VIEW HOMES LLC TRN: 2149832472TC</t>
+          <t>CHECK # 1012</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>-1383.06</v>
+        <v>-32224</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -6126,7 +6126,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Exp-Mortgage</t>
+          <t>Exp-Insurance</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -6136,7 +6136,7 @@
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>4920Brianhill</t>
+          <t>Midway</t>
         </is>
       </c>
       <c r="K88" t="inlineStr">
@@ -6146,33 +6146,33 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>Insurance</t>
         </is>
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>Midway</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>4920Brianhill</t>
+          <t>104Meadow</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2024-07-31</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:073124 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926084765326 EED:240731   IND ID:QZKLM2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 2134765326TC</t>
+          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VMZ9B 104MV TO TRULO PROPERTY MANAGEMENT</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>6414.53</v>
+        <v>-75</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -6191,17 +6191,17 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-Mgmt</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>4920Brianhill</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>104Meadow</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
@@ -6211,33 +6211,33 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>W9-TRULO</t>
         </is>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>PropertyManagement</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>4920Brianhill</t>
+          <t>114Sidney</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:JPMORGAN CHASE         ORIG ID:1000008113 DESC DATE:070124 CO ENTRY DESCR:CHASE ACH SEC:PPD    TRACE#:021000020928596 EED:240701   IND ID:                             IND NAME:MEADOW VIEW HOMES LLC TRN: 1830928596TC</t>
+          <t>ORIG CO NAME:SERVICEMAC PMT         ORIG ID:4823070213 DESC DATE:080124 CO ENTRY DESCR:MTGE PAYMTSEC:PPD    TRACE#:091000019427854 EED:240801   IND ID:                             IND NAME:PARUL GUPTA TRN: 2149427854TC</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>-1383.06</v>
+        <v>-675.63</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -6266,7 +6266,7 @@
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>4920Brianhill</t>
+          <t>114Sidney</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
@@ -6288,21 +6288,21 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>8604Wagon</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-05</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:PENNYMAC               ORIG ID:1262049351 DESC DATE:Aug 24 CO ENTRY DESCR:CASH      SEC:WEB    TRACE#:021000021437718 EED:240801   IND ID:8028351082-0056              IND NAME:8604 Wagon TRN: 2141437718TC</t>
+          <t>ONLINE TRANSFER FROM GUPTA P REF #IB0PGKBTSH PLATINUM SAVINGS EDDY ESTATES JUL AUG MORTGAGE</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>-843.79</v>
+        <v>1894.9</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -6326,12 +6326,12 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>8604Wagon</t>
+          <t>GeneralCustomer</t>
         </is>
       </c>
       <c r="K91" t="inlineStr">
@@ -6341,33 +6341,33 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>GeneralVendor</t>
+          <t>1905Morning</t>
         </is>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>Mortgage</t>
+          <t>EddyEstatesLLC</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-09-06</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VK6BX TRULO MONTHLY PM FEE MIDWAY INN</t>
+          <t>ORIG CO NAME:CITY OF FORT WOR       ORIG ID:0000000160 DESC DATE:240905 CO ENTRY DESCR:BILLPAY   SEC:PPD    TRACE#:091000017273188 EED:240906   IND ID:                             IND NAME:NEERAJ GUPTA TRN: 2507273188TC</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>-1500</v>
+        <v>-48.89</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -6386,17 +6386,17 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Exp-Utilities</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Midway</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="K92" t="inlineStr">
@@ -6406,33 +6406,33 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M92" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>CityServices</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>1342Newton</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-15</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ6T9P2 NEWTON TO TRULO PROPERTY MANAGEMENT</t>
+          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:081524 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926085820474 EED:240815   IND ID:4DRRN2                       IND NAME:Pagoda Homes LLC (Jame                                                                                       469-867-9837 TRN: 2285820474TC</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>-75</v>
+        <v>2239.53</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -6451,17 +6451,17 @@
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>4909Jamesway</t>
         </is>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>1342Newton</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
@@ -6471,33 +6471,33 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>104Meadow</t>
+          <t>114Sidney</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2024-08-01</t>
+          <t>2024-08-09</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0P2VMZ9B 104MV TO TRULO PROPERTY MANAGEMENT</t>
+          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:080924 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926082370597 EED:240809   IND ID:ZY88N2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 2222370597TC</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>-75</v>
+        <v>1644.72</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -6516,17 +6516,17 @@
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Rev-Rent</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>114Sidney</t>
         </is>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>104Meadow</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
@@ -6536,33 +6536,33 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>6401Basswood</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-09-03</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>RECURRING TRANSFER TO JPMORGAN CHASE BANK, NA CHK XXXXX8616 N. GUPTA REF #FP0NQ59Q3N BREWER TO TRULO PROPERTY MANAGEMENT</t>
+          <t>ORIG CO NAME:NEWREZ-SHELLPOIN       ORIG ID:6371542226 DESC DATE:240831 CO ENTRY DESCR:ACH PMT   SEC:PPD    TRACE#:028000086173075 EED:240903   IND ID:                             IND NAME:JADHAV VIVEK TRN: 2476173075TC</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>-75</v>
+        <v>-1383.06</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -6581,17 +6581,17 @@
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Exp-Mgmt</t>
+          <t>Exp-Mortgage</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>1117Brewer</t>
+          <t>6401Basswood</t>
         </is>
       </c>
       <c r="K95" t="inlineStr">
@@ -6601,33 +6601,33 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>W9-TRULO</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>PropertyManagement</t>
+          <t>Mortgage</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>6401Basswood</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2024-07-22</t>
+          <t>2024-08-15</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:VRBO                   ORIG ID:9872667522 DESC DATE:240719 CO ENTRY DESCR:PAYMENT   SEC:PPD    TRACE#:031101111714572 EED:240722   IND ID:                             IND NAME:Neeraj Gupta TRN: 2041714572TC</t>
+          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:081524 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926085820469 EED:240815   IND ID:VCRRN2                       IND NAME:Pagoda Homes LLC (Bass                                                                                       469-867-9837 TRN: 2285820469TC</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>1699.24</v>
+        <v>2850.41</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -6651,12 +6651,12 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>4909Jamesway</t>
+          <t>6401Basswood</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -6666,33 +6666,33 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>VRBORent</t>
+          <t>Property</t>
         </is>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>GeneralCustomer</t>
+          <t>W9-ONEPLUS</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>8604Wagon</t>
+          <t>6401Basswood</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2024-07-10</t>
+          <t>2024-08-12</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:071024 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088315745 EED:240710   IND ID:9TRBL2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 1928315745TC</t>
+          <t xml:space="preserve">CHECK 1071  </t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>2100</v>
+        <v>-50</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -6711,17 +6711,17 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Rev-Rent</t>
+          <t>Exp-ProfessionalServices</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>8604Wagon</t>
+          <t>GeneralVendor</t>
         </is>
       </c>
       <c r="J97" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>6401Basswood</t>
         </is>
       </c>
       <c r="K97" t="inlineStr">
@@ -6731,33 +6731,33 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>CityofFortworthViolation</t>
         </is>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>W9-ONEPLUS</t>
+          <t>6401Basswood</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>8604Wagon</t>
+          <t>6401Basswood</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2024-07-01</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>ORIG CO NAME:PENNYMAC               ORIG ID:1262049351 DESC DATE:Jul 24 CO ENTRY DESCR:CASH      SEC:WEB    TRACE#:021000020542007 EED:240701   IND ID:8028351082-0055              IND NAME:8604 Wagon TRN: 1830542007TC</t>
+          <t>ORIG CO NAME:NEWREZ-SHELLPOIN       ORIG ID:6371542226 DESC DATE:240731 CO ENTRY DESCR:ACH PMT   SEC:PPD    TRACE#:028000083659872 EED:240801   IND ID:                             IND NAME:JADHAV VIVEK TRN: 2143659872TC</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>-843.79</v>
+        <v>-1383.06</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -6786,7 +6786,7 @@
       </c>
       <c r="J98" t="inlineStr">
         <is>
-          <t>8604Wagon</t>
+          <t>6401Basswood</t>
         </is>
       </c>
       <c r="K98" t="inlineStr">
@@ -6800,396 +6800,6 @@
         </is>
       </c>
       <c r="M98" t="inlineStr">
-        <is>
-          <t>Mortgage</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>114Sidney</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>ORIG CO NAME:SERVICEMAC PMT         ORIG ID:4823070213 DESC DATE:080124 CO ENTRY DESCR:MTGE PAYMTSEC:PPD    TRACE#:091000019427854 EED:240801   IND ID:                             IND NAME:PARUL GUPTA TRN: 2149427854TC</t>
-        </is>
-      </c>
-      <c r="D99" t="n">
-        <v>-675.63</v>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>clean</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>A01-Income</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t>Exp-Mortgage</t>
-        </is>
-      </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>GeneralVendor</t>
-        </is>
-      </c>
-      <c r="J99" t="inlineStr">
-        <is>
-          <t>114Sidney</t>
-        </is>
-      </c>
-      <c r="K99" t="inlineStr">
-        <is>
-          <t>Initial</t>
-        </is>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>GeneralVendor</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
-          <t>Mortgage</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>114Sidney</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>2024-07-10</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:071024 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088315744 EED:240710   IND ID:8TRBL2                       IND NAME:Meadow View Homes LLC                                                                                        469-867-9837 TRN: 1928315744TC</t>
-        </is>
-      </c>
-      <c r="D100" t="n">
-        <v>1860</v>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>clean</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>A01-Income</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t>Rev-Rent</t>
-        </is>
-      </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>114Sidney</t>
-        </is>
-      </c>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>W9-ONEPLUS</t>
-        </is>
-      </c>
-      <c r="K100" t="inlineStr">
-        <is>
-          <t>Initial</t>
-        </is>
-      </c>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>Property</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr">
-        <is>
-          <t>W9-ONEPLUS</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>114Sidney</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>2024-07-01</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>ORIG CO NAME:SERVICEMAC PMT         ORIG ID:4823070213 DESC DATE:070124 CO ENTRY DESCR:MTGE PAYMTSEC:PPD    TRACE#:091000010669125 EED:240701   IND ID:                             IND NAME:PARUL GUPTA TRN: 1830669125TC</t>
-        </is>
-      </c>
-      <c r="D101" t="n">
-        <v>-675.63</v>
-      </c>
-      <c r="E101" t="inlineStr">
-        <is>
-          <t>clean</t>
-        </is>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="G101" t="inlineStr">
-        <is>
-          <t>A01-Income</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t>Exp-Mortgage</t>
-        </is>
-      </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>GeneralVendor</t>
-        </is>
-      </c>
-      <c r="J101" t="inlineStr">
-        <is>
-          <t>114Sidney</t>
-        </is>
-      </c>
-      <c r="K101" t="inlineStr">
-        <is>
-          <t>Initial</t>
-        </is>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>GeneralVendor</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
-          <t>Mortgage</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>6401Basswood</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>2024-08-01</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>ORIG CO NAME:NEWREZ-SHELLPOIN       ORIG ID:6371542226 DESC DATE:240731 CO ENTRY DESCR:ACH PMT   SEC:PPD    TRACE#:028000083659872 EED:240801   IND ID:                             IND NAME:JADHAV VIVEK TRN: 2143659872TC</t>
-        </is>
-      </c>
-      <c r="D102" t="n">
-        <v>-1383.06</v>
-      </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>clean</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>A01-Income</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t>Exp-Mortgage</t>
-        </is>
-      </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>GeneralVendor</t>
-        </is>
-      </c>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>6401Basswood</t>
-        </is>
-      </c>
-      <c r="K102" t="inlineStr">
-        <is>
-          <t>Initial</t>
-        </is>
-      </c>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t>GeneralVendor</t>
-        </is>
-      </c>
-      <c r="M102" t="inlineStr">
-        <is>
-          <t>Mortgage</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>6401Basswood</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>2024-07-10</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>ORIG CO NAME:OnePlus Realty G       ORIG ID:9001504486 DESC DATE:071024 CO ENTRY DESCR:SIGONFILE SEC:CCD    TRACE#:111926088315742 EED:240710   IND ID:ZSRBL2                       IND NAME:Pagoda Homes LLC (Bass                                                                                       469-867-9837 TRN: 1928315742TC</t>
-        </is>
-      </c>
-      <c r="D103" t="n">
-        <v>2655</v>
-      </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>clean</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>A01-Income</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t>Rev-Rent</t>
-        </is>
-      </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>6401Basswood</t>
-        </is>
-      </c>
-      <c r="J103" t="inlineStr">
-        <is>
-          <t>W9-ONEPLUS</t>
-        </is>
-      </c>
-      <c r="K103" t="inlineStr">
-        <is>
-          <t>Initial</t>
-        </is>
-      </c>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>Property</t>
-        </is>
-      </c>
-      <c r="M103" t="inlineStr">
-        <is>
-          <t>W9-ONEPLUS</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>6401Basswood</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>2024-07-01</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>ORIG CO NAME:NEWREZ-SHELLPOIN       ORIG ID:6371542226 DESC DATE:240630 CO ENTRY DESCR:ACH PMT   SEC:PPD    TRACE#:028000083248476 EED:240701   IND ID:                             IND NAME:JADHAV VIVEK TRN: 1833248476TC</t>
-        </is>
-      </c>
-      <c r="D104" t="n">
-        <v>-1383.06</v>
-      </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t>clean</t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>open</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>A01-Income</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t>Exp-Mortgage</t>
-        </is>
-      </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>GeneralVendor</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>6401Basswood</t>
-        </is>
-      </c>
-      <c r="K104" t="inlineStr">
-        <is>
-          <t>Initial</t>
-        </is>
-      </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>GeneralVendor</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr">
         <is>
           <t>Mortgage</t>
         </is>

</xml_diff>